<commit_message>
Corrige nome da coluna para NOME na planilha
</commit_message>
<xml_diff>
--- a/04. Farol.xlsx
+++ b/04. Farol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefferson.araujo\Downloads\bot_telegram_webhook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A2EAE2-E4DD-41DA-975A-B13843B2849E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75816174-ED7F-4594-B2FC-BDBD2E40E19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0594B627-261B-49DD-877B-E559C01B3B93}"/>
   </bookViews>
@@ -1569,7 +1569,7 @@
     <t>Login</t>
   </si>
   <si>
-    <t>Nome</t>
+    <t>NOME</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Corrige nomes de colunas para Data e TOTAL conforme planilha
</commit_message>
<xml_diff>
--- a/04. Farol.xlsx
+++ b/04. Farol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefferson.araujo\Downloads\bot_telegram_webhook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75816174-ED7F-4594-B2FC-BDBD2E40E19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A2EAE2-E4DD-41DA-975A-B13843B2849E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0594B627-261B-49DD-877B-E559C01B3B93}"/>
   </bookViews>
@@ -1569,7 +1569,7 @@
     <t>Login</t>
   </si>
   <si>
-    <t>NOME</t>
+    <t>Nome</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Atualiza planilha de RV
</commit_message>
<xml_diff>
--- a/04. Farol.xlsx
+++ b/04. Farol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jefferson.araujo\Downloads\bot_telegram_webhook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1518A615-FA24-4B43-9407-21C30D1EC3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48BB2CCB-5D2E-4296-9280-2D19BD815D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0594B627-261B-49DD-877B-E559C01B3B93}"/>
   </bookViews>
@@ -4681,7 +4681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF0DB9DD-757A-4456-AE79-B218C28D70D1}">
   <dimension ref="A1:AH1343"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A654" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A662" sqref="A662:R1343"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -60288,7 +60290,7 @@
         <v>0</v>
       </c>
       <c r="M774" s="6">
-        <v>0</v>
+        <v>16.75</v>
       </c>
       <c r="N774" s="6">
         <v>0</v>
@@ -60303,7 +60305,7 @@
         <v>0</v>
       </c>
       <c r="R774" s="4">
-        <v>0</v>
+        <v>16.75</v>
       </c>
       <c r="S774" s="1" t="s">
         <v>519</v>
@@ -62489,7 +62491,7 @@
         <v>0</v>
       </c>
       <c r="M805" s="6">
-        <v>0</v>
+        <v>20.9</v>
       </c>
       <c r="N805" s="6">
         <v>0</v>
@@ -62504,7 +62506,7 @@
         <v>0</v>
       </c>
       <c r="R805" s="4">
-        <v>0</v>
+        <v>20.9</v>
       </c>
       <c r="S805" s="1" t="s">
         <v>519</v>
@@ -64690,7 +64692,7 @@
         <v>0</v>
       </c>
       <c r="M836" s="6">
-        <v>0</v>
+        <v>19.03</v>
       </c>
       <c r="N836" s="6">
         <v>0</v>
@@ -64705,7 +64707,7 @@
         <v>0</v>
       </c>
       <c r="R836" s="4">
-        <v>0</v>
+        <v>19.03</v>
       </c>
       <c r="S836" s="1" t="s">
         <v>519</v>
@@ -71293,7 +71295,7 @@
         <v>0</v>
       </c>
       <c r="M929" s="6">
-        <v>0</v>
+        <v>14.88</v>
       </c>
       <c r="N929" s="6">
         <v>0</v>
@@ -71308,7 +71310,7 @@
         <v>0</v>
       </c>
       <c r="R929" s="4">
-        <v>0</v>
+        <v>14.88</v>
       </c>
       <c r="S929" s="1" t="s">
         <v>519</v>
@@ -73494,7 +73496,7 @@
         <v>0</v>
       </c>
       <c r="M960" s="6">
-        <v>0</v>
+        <v>18.940000000000001</v>
       </c>
       <c r="N960" s="6">
         <v>0</v>
@@ -73509,7 +73511,7 @@
         <v>0</v>
       </c>
       <c r="R960" s="4">
-        <v>0</v>
+        <v>18.940000000000001</v>
       </c>
       <c r="S960" s="1" t="s">
         <v>519</v>
@@ -75695,7 +75697,7 @@
         <v>0</v>
       </c>
       <c r="M991" s="6">
-        <v>0</v>
+        <v>16.510000000000002</v>
       </c>
       <c r="N991" s="6">
         <v>0</v>
@@ -75710,7 +75712,7 @@
         <v>0</v>
       </c>
       <c r="R991" s="4">
-        <v>0</v>
+        <v>16.510000000000002</v>
       </c>
       <c r="S991" s="1" t="s">
         <v>519</v>
@@ -80097,7 +80099,7 @@
         <v>0</v>
       </c>
       <c r="M1053" s="6">
-        <v>0</v>
+        <v>17.63</v>
       </c>
       <c r="N1053" s="6">
         <v>0</v>
@@ -80112,7 +80114,7 @@
         <v>0</v>
       </c>
       <c r="R1053" s="4">
-        <v>0</v>
+        <v>17.63</v>
       </c>
       <c r="S1053" s="1" t="e">
         <v>#N/A</v>
@@ -82298,7 +82300,7 @@
         <v>0</v>
       </c>
       <c r="M1084" s="6">
-        <v>0</v>
+        <v>19.64</v>
       </c>
       <c r="N1084" s="6">
         <v>0</v>
@@ -82313,7 +82315,7 @@
         <v>0</v>
       </c>
       <c r="R1084" s="4">
-        <v>0</v>
+        <v>19.64</v>
       </c>
       <c r="S1084" s="1" t="e">
         <v>#N/A</v>
@@ -84499,7 +84501,7 @@
         <v>0</v>
       </c>
       <c r="M1115" s="6">
-        <v>0</v>
+        <v>20.93</v>
       </c>
       <c r="N1115" s="6">
         <v>0</v>
@@ -84514,7 +84516,7 @@
         <v>0</v>
       </c>
       <c r="R1115" s="4">
-        <v>0</v>
+        <v>20.93</v>
       </c>
       <c r="S1115" s="1" t="e">
         <v>#N/A</v>

</xml_diff>